<commit_message>
ws office open bug fixed
</commit_message>
<xml_diff>
--- a/examples/simple.xlsx
+++ b/examples/simple.xlsx
@@ -6,9 +6,9 @@
   <bookViews>
     <workbookView showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="204" windowHeight="8192" windowWidth="16384" xWindow="0" yWindow="0"/>
   </bookViews>
-  <calcPr iterate="0" iterateCount="100" iterateDelta="0.001" refMode="A1"/>
+  <calcPr iterateCount="100" iterate="0" iterateDelta="0.001" refMode="A1"/>
   <sheets>
-    <sheet name="Sheet1" r:id="rId1" sheetId="1" state="visible"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1" state="visible"/>
   </sheets>
 </workbook>
 </file>
@@ -61,16 +61,16 @@
     </border>
   </borders>
   <cellXfs count="4">
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="0" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="0" applyFill="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="0" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFill="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="2" fontId="0" numFmtId="0">
       <alignment horizontal="center" indent="0" shrinkToFit="0" textRotation="0" vertical="center" wrapText="0"/>
     </xf>
-    <xf applyAlignment="0" applyBorder="1" applyFill="0" applyFont="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="0" numFmtId="0">
+    <xf applyAlignment="0" applyBorder="1" applyFont="0" applyFill="0" applyNumberFormat="0" applyProtection="0" borderId="1" fillId="0" fontId="0" numFmtId="0">
       <alignment horizontal="general" indent="0" shrinkToFit="0" textRotation="0" vertical="bottom" wrapText="0"/>
     </xf>
   </cellXfs>
@@ -408,9 +408,9 @@
       <selection activeCell="A1" activeCellId="0" pane="topLeft" sqref="A1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="0" defaultRowHeight="12.85"/>
+  <sheetFormatPr defaultRowHeight="12.85" defaultColWidth="0"/>
   <printOptions gridLines="0" gridLinesSet="1" headings="0" horizontalCentered="0" verticalCentered="0"/>
-  <pageMargins bottom="1.05277777777778" footer="0.7875" header="0.7875" left="0.7875" right="0.7875" top="1.05277777777778"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup blackAndWhite="0" cellComments="none" copies="1" draft="0" firstPageNumber="1" fitToHeight="1" fitToWidth="1" horizontalDpi="300" orientation="portrait" pageOrder="downThenOver" paperSize="9" scale="100" useFirstPageNumber="1" usePrinterDefaults="0" verticalDpi="300"/>
   <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
@@ -421,22 +421,22 @@
   </mergeCells>
   <dimension ref="A1:C2"/>
   <cols>
-    <col collapsed="0" customWidth="0" hidden="0" max="1" min="1" outlineLevel="0" style="1" width="9.5"/>
-    <col collapsed="0" customWidth="0" hidden="0" max="2" min="2" outlineLevel="0" style="1" width="9.5"/>
-    <col collapsed="0" customWidth="0" hidden="0" max="3" min="3" outlineLevel="0" style="1" width="9.5"/>
+    <col min="1" max="1" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="1"/>
+    <col min="2" max="2" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="1"/>
+    <col min="3" max="3" hidden="0" width="9.5" customWidth="0" collapsed="0" outlineLevel="0" style="1"/>
   </cols>
   <sheetData>
-    <row outlineLevel="0" r="1">
-      <c r="A1" s="2" t="s">
+    <row r="1" outlineLevel="0">
+      <c r="A1" t="s" s="2">
         <v>0</v>
       </c>
-      <c r="B1" s="3" t="s"/>
-      <c r="C1" s="3" t="s"/>
+      <c r="B1" t="s" s="3"/>
+      <c r="C1" t="s" s="3"/>
     </row>
-    <row outlineLevel="0" r="2">
-      <c r="A2" s="3" t="s"/>
-      <c r="B2" s="3" t="s"/>
-      <c r="C2" s="3" t="s"/>
+    <row r="2" outlineLevel="0">
+      <c r="A2" t="s" s="3"/>
+      <c r="B2" t="s" s="3"/>
+      <c r="C2" t="s" s="3"/>
     </row>
   </sheetData>
 </worksheet>

</xml_diff>